<commit_message>
edits to nightly code
</commit_message>
<xml_diff>
--- a/Ecobat_ProForma.xlsx
+++ b/Ecobat_ProForma.xlsx
@@ -770,7 +770,7 @@
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
-          <t>OPTIONAL</t>
+          <t>REQUIRED</t>
         </r>
         <r>
           <rPr>
@@ -792,7 +792,8 @@
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
-          <t>The number of bats of this species identifiable at the same pass period. Usually 1.</t>
+          <t>The number of bats of this species identifiable at the same pass period (often 1).
+When uploading the data, if you receive and error for this column, please ensure it is formatted as a Number with 0 decimal places.</t>
         </r>
       </text>
     </comment>
@@ -2225,7 +2226,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -2492,7 +2493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2524,15 +2525,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2544,20 +2536,17 @@
     <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2567,11 +2556,24 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2862,49 +2864,49 @@
   <dimension ref="A1:AI257"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="AE34" sqref="AE34"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" style="20" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="20" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="20" customWidth="1"/>
+    <col min="1" max="1" width="16" style="17" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="17" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" style="11" customWidth="1"/>
-    <col min="7" max="7" width="25" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" style="24" customWidth="1"/>
-    <col min="9" max="9" width="10" style="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="20" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" style="20" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="24"/>
-    <col min="14" max="14" width="13.42578125" style="20" customWidth="1"/>
-    <col min="15" max="15" width="15.7109375" style="20" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="20"/>
-    <col min="18" max="18" width="13.5703125" style="20" customWidth="1"/>
-    <col min="19" max="19" width="14.85546875" style="20" customWidth="1"/>
-    <col min="20" max="20" width="11.7109375" style="24" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" style="20"/>
-    <col min="22" max="22" width="11.5703125" style="24" customWidth="1"/>
-    <col min="23" max="23" width="13.42578125" style="20" customWidth="1"/>
-    <col min="24" max="27" width="9.140625" style="20"/>
+    <col min="7" max="7" width="25" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="31" customWidth="1"/>
+    <col min="9" max="9" width="10" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="17" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" style="17" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="20"/>
+    <col min="14" max="14" width="13.42578125" style="17" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" style="17" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" style="17"/>
+    <col min="18" max="18" width="13.5703125" style="17" customWidth="1"/>
+    <col min="19" max="19" width="14.85546875" style="17" customWidth="1"/>
+    <col min="20" max="20" width="11.7109375" style="20" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" style="17"/>
+    <col min="22" max="22" width="11.5703125" style="20" customWidth="1"/>
+    <col min="23" max="23" width="13.42578125" style="17" customWidth="1"/>
+    <col min="24" max="27" width="9.140625" style="17"/>
     <col min="32" max="32" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="15" t="s">
         <v>64</v>
       </c>
       <c r="E1" s="13" t="s">
@@ -2913,270 +2915,270 @@
       <c r="F1" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="K1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="L1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="29" t="s">
+      <c r="N1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="30" t="s">
+      <c r="O1" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="29" t="s">
+      <c r="P1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="31" t="s">
+      <c r="Q1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="29" t="s">
+      <c r="R1" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="30" t="s">
+      <c r="S1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="27" t="s">
+      <c r="T1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="29" t="s">
+      <c r="U1" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="V1" s="32" t="s">
+      <c r="V1" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="W1" s="29" t="s">
+      <c r="W1" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="X1" s="33" t="s">
+      <c r="X1" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="Y1" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="Z1" s="16"/>
-      <c r="AA1" s="17"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="34"/>
       <c r="AB1" s="4"/>
       <c r="AG1" s="5"/>
       <c r="AH1" s="6"/>
       <c r="AI1" s="6"/>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
+      <c r="A2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
       <c r="AB2" s="6"/>
       <c r="AG2" s="7"/>
       <c r="AH2" s="6"/>
       <c r="AI2" s="6"/>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
       <c r="AB3" s="6"/>
       <c r="AG3" s="7"/>
       <c r="AH3" s="6"/>
       <c r="AI3" s="6"/>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
       <c r="AB4" s="6"/>
       <c r="AG4" s="7"/>
       <c r="AH4" s="6"/>
       <c r="AI4" s="6"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
       <c r="AB5" s="6"/>
       <c r="AG5" s="7"/>
       <c r="AH5" s="6"/>
       <c r="AI5" s="6"/>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="19"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
       <c r="AB6" s="6"/>
       <c r="AG6" s="7"/>
       <c r="AH6" s="6"/>
       <c r="AI6" s="6"/>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="19"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
       <c r="AB7" s="6"/>
       <c r="AG7" s="7"/>
       <c r="AH7" s="6"/>
       <c r="AI7" s="6"/>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
       <c r="AB8" s="6"/>
       <c r="AG8" s="7"/>
       <c r="AH8" s="6"/>
       <c r="AI8" s="6"/>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
       <c r="AB9" s="6"/>
       <c r="AG9" s="7"/>
       <c r="AH9" s="6"/>
       <c r="AI9" s="6"/>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
       <c r="AB10" s="6"/>
       <c r="AG10" s="6"/>
       <c r="AH10" s="6"/>
       <c r="AI10" s="6"/>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
       <c r="AB11" s="6"/>
       <c r="AG11" s="6"/>
       <c r="AH11" s="6"/>
       <c r="AI11" s="6"/>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
       <c r="AB12" s="6"/>
       <c r="AG12" s="6"/>
       <c r="AH12" s="6"/>
       <c r="AI12" s="6"/>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="N13" s="19"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
-      <c r="Q13" s="19"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
       <c r="AB13" s="6"/>
       <c r="AC13" s="6"/>
       <c r="AD13" s="6"/>
@@ -3187,18 +3189,18 @@
       <c r="AI13" s="6"/>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="N14" s="19"/>
-      <c r="O14" s="19"/>
-      <c r="P14" s="19"/>
-      <c r="Q14" s="19"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
       <c r="AB14" s="6"/>
       <c r="AC14" s="6"/>
       <c r="AD14" s="6"/>
@@ -3209,16 +3211,16 @@
       <c r="AI14" s="6"/>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="N15" s="19"/>
-      <c r="O15" s="19"/>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="19"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
       <c r="AB15" s="6"/>
       <c r="AC15" s="6"/>
       <c r="AD15" s="6"/>
@@ -3229,18 +3231,18 @@
       <c r="AI15" s="6"/>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
-      <c r="N16" s="19"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="19"/>
-      <c r="Q16" s="19"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
       <c r="AB16" s="6"/>
       <c r="AC16" s="6"/>
       <c r="AD16" s="6"/>
@@ -3251,16 +3253,16 @@
       <c r="AI16" s="6"/>
     </row>
     <row r="17" spans="3:35" x14ac:dyDescent="0.25">
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="N17" s="19"/>
-      <c r="O17" s="19"/>
-      <c r="P17" s="19"/>
-      <c r="Q17" s="19"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
       <c r="AB17" s="6"/>
       <c r="AC17" s="6"/>
       <c r="AD17" s="6"/>
@@ -3271,856 +3273,856 @@
       <c r="AI17" s="6"/>
     </row>
     <row r="18" spans="3:35" x14ac:dyDescent="0.25">
-      <c r="P18" s="19"/>
-      <c r="Q18" s="19"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
     </row>
     <row r="19" spans="3:35" x14ac:dyDescent="0.25">
-      <c r="P19" s="19"/>
-      <c r="Q19" s="19"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="16"/>
     </row>
     <row r="20" spans="3:35" x14ac:dyDescent="0.25">
-      <c r="P20" s="19"/>
-      <c r="Q20" s="19"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
     </row>
     <row r="21" spans="3:35" x14ac:dyDescent="0.25">
-      <c r="P21" s="19"/>
-      <c r="Q21" s="19"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
     </row>
     <row r="22" spans="3:35" x14ac:dyDescent="0.25">
-      <c r="P22" s="19"/>
-      <c r="Q22" s="19"/>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="16"/>
     </row>
     <row r="23" spans="3:35" x14ac:dyDescent="0.25">
-      <c r="P23" s="19"/>
-      <c r="Q23" s="19"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="16"/>
     </row>
     <row r="24" spans="3:35" x14ac:dyDescent="0.25">
-      <c r="P24" s="19"/>
-      <c r="Q24" s="19"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
     </row>
     <row r="25" spans="3:35" x14ac:dyDescent="0.25">
-      <c r="P25" s="19"/>
-      <c r="Q25" s="19"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="16"/>
     </row>
     <row r="26" spans="3:35" x14ac:dyDescent="0.25">
-      <c r="P26" s="19"/>
-      <c r="Q26" s="19"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="16"/>
     </row>
     <row r="27" spans="3:35" x14ac:dyDescent="0.25">
-      <c r="P27" s="19"/>
-      <c r="Q27" s="19"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="16"/>
     </row>
     <row r="28" spans="3:35" x14ac:dyDescent="0.25">
-      <c r="P28" s="19"/>
-      <c r="Q28" s="19"/>
+      <c r="P28" s="16"/>
+      <c r="Q28" s="16"/>
     </row>
     <row r="29" spans="3:35" x14ac:dyDescent="0.25">
-      <c r="P29" s="19"/>
-      <c r="Q29" s="19"/>
+      <c r="P29" s="16"/>
+      <c r="Q29" s="16"/>
     </row>
     <row r="30" spans="3:35" x14ac:dyDescent="0.25">
-      <c r="P30" s="19"/>
-      <c r="Q30" s="19"/>
+      <c r="P30" s="16"/>
+      <c r="Q30" s="16"/>
     </row>
     <row r="31" spans="3:35" x14ac:dyDescent="0.25">
-      <c r="P31" s="19"/>
-      <c r="Q31" s="19"/>
+      <c r="P31" s="16"/>
+      <c r="Q31" s="16"/>
     </row>
     <row r="32" spans="3:35" x14ac:dyDescent="0.25">
-      <c r="P32" s="19"/>
-      <c r="Q32" s="19"/>
+      <c r="P32" s="16"/>
+      <c r="Q32" s="16"/>
     </row>
     <row r="33" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P33" s="19"/>
+      <c r="P33" s="16"/>
     </row>
     <row r="34" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P34" s="19"/>
+      <c r="P34" s="16"/>
     </row>
     <row r="35" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P35" s="19"/>
+      <c r="P35" s="16"/>
     </row>
     <row r="36" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P36" s="19"/>
+      <c r="P36" s="16"/>
     </row>
     <row r="37" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P37" s="19"/>
+      <c r="P37" s="16"/>
     </row>
     <row r="38" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P38" s="19"/>
+      <c r="P38" s="16"/>
     </row>
     <row r="39" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P39" s="19"/>
-      <c r="R39" s="19"/>
+      <c r="P39" s="16"/>
+      <c r="R39" s="16"/>
     </row>
     <row r="40" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P40" s="19"/>
-      <c r="R40" s="19"/>
+      <c r="P40" s="16"/>
+      <c r="R40" s="16"/>
     </row>
     <row r="41" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P41" s="19"/>
-      <c r="R41" s="19"/>
+      <c r="P41" s="16"/>
+      <c r="R41" s="16"/>
     </row>
     <row r="42" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P42" s="19"/>
-      <c r="R42" s="19"/>
+      <c r="P42" s="16"/>
+      <c r="R42" s="16"/>
     </row>
     <row r="43" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P43" s="19"/>
-      <c r="R43" s="19"/>
+      <c r="P43" s="16"/>
+      <c r="R43" s="16"/>
     </row>
     <row r="44" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P44" s="19"/>
-      <c r="R44" s="19"/>
+      <c r="P44" s="16"/>
+      <c r="R44" s="16"/>
     </row>
     <row r="45" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P45" s="19"/>
-      <c r="R45" s="19"/>
+      <c r="P45" s="16"/>
+      <c r="R45" s="16"/>
     </row>
     <row r="46" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P46" s="19"/>
-      <c r="R46" s="19"/>
+      <c r="P46" s="16"/>
+      <c r="R46" s="16"/>
     </row>
     <row r="47" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P47" s="19"/>
-      <c r="R47" s="19"/>
+      <c r="P47" s="16"/>
+      <c r="R47" s="16"/>
     </row>
     <row r="48" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P48" s="19"/>
-      <c r="R48" s="19"/>
+      <c r="P48" s="16"/>
+      <c r="R48" s="16"/>
     </row>
     <row r="49" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P49" s="19"/>
-      <c r="R49" s="19"/>
+      <c r="P49" s="16"/>
+      <c r="R49" s="16"/>
     </row>
     <row r="50" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P50" s="19"/>
-      <c r="R50" s="19"/>
+      <c r="P50" s="16"/>
+      <c r="R50" s="16"/>
     </row>
     <row r="51" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P51" s="19"/>
-      <c r="R51" s="19"/>
+      <c r="P51" s="16"/>
+      <c r="R51" s="16"/>
     </row>
     <row r="52" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P52" s="19"/>
-      <c r="R52" s="19"/>
+      <c r="P52" s="16"/>
+      <c r="R52" s="16"/>
     </row>
     <row r="53" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P53" s="19"/>
-      <c r="R53" s="19"/>
+      <c r="P53" s="16"/>
+      <c r="R53" s="16"/>
     </row>
     <row r="54" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P54" s="19"/>
-      <c r="R54" s="19"/>
+      <c r="P54" s="16"/>
+      <c r="R54" s="16"/>
     </row>
     <row r="55" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P55" s="19"/>
-      <c r="R55" s="19"/>
+      <c r="P55" s="16"/>
+      <c r="R55" s="16"/>
     </row>
     <row r="56" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P56" s="19"/>
-      <c r="R56" s="19"/>
+      <c r="P56" s="16"/>
+      <c r="R56" s="16"/>
     </row>
     <row r="57" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P57" s="19"/>
-      <c r="R57" s="19"/>
+      <c r="P57" s="16"/>
+      <c r="R57" s="16"/>
     </row>
     <row r="58" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P58" s="19"/>
-      <c r="R58" s="19"/>
+      <c r="P58" s="16"/>
+      <c r="R58" s="16"/>
     </row>
     <row r="59" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P59" s="19"/>
-      <c r="R59" s="19"/>
+      <c r="P59" s="16"/>
+      <c r="R59" s="16"/>
     </row>
     <row r="60" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P60" s="19"/>
-      <c r="R60" s="19"/>
+      <c r="P60" s="16"/>
+      <c r="R60" s="16"/>
     </row>
     <row r="61" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P61" s="19"/>
-      <c r="R61" s="19"/>
+      <c r="P61" s="16"/>
+      <c r="R61" s="16"/>
     </row>
     <row r="62" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P62" s="19"/>
-      <c r="R62" s="19"/>
+      <c r="P62" s="16"/>
+      <c r="R62" s="16"/>
     </row>
     <row r="63" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P63" s="19"/>
-      <c r="R63" s="19"/>
+      <c r="P63" s="16"/>
+      <c r="R63" s="16"/>
     </row>
     <row r="64" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P64" s="19"/>
-      <c r="R64" s="19"/>
+      <c r="P64" s="16"/>
+      <c r="R64" s="16"/>
     </row>
     <row r="65" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P65" s="19"/>
-      <c r="R65" s="19"/>
+      <c r="P65" s="16"/>
+      <c r="R65" s="16"/>
     </row>
     <row r="66" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P66" s="19"/>
-      <c r="R66" s="19"/>
+      <c r="P66" s="16"/>
+      <c r="R66" s="16"/>
     </row>
     <row r="67" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P67" s="19"/>
-      <c r="R67" s="19"/>
+      <c r="P67" s="16"/>
+      <c r="R67" s="16"/>
     </row>
     <row r="68" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P68" s="19"/>
-      <c r="R68" s="19"/>
+      <c r="P68" s="16"/>
+      <c r="R68" s="16"/>
     </row>
     <row r="69" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P69" s="19"/>
-      <c r="R69" s="19"/>
+      <c r="P69" s="16"/>
+      <c r="R69" s="16"/>
     </row>
     <row r="70" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P70" s="19"/>
-      <c r="R70" s="19"/>
+      <c r="P70" s="16"/>
+      <c r="R70" s="16"/>
     </row>
     <row r="71" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P71" s="19"/>
-      <c r="R71" s="19"/>
+      <c r="P71" s="16"/>
+      <c r="R71" s="16"/>
     </row>
     <row r="72" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P72" s="19"/>
-      <c r="R72" s="19"/>
+      <c r="P72" s="16"/>
+      <c r="R72" s="16"/>
     </row>
     <row r="73" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P73" s="19"/>
-      <c r="R73" s="19"/>
+      <c r="P73" s="16"/>
+      <c r="R73" s="16"/>
     </row>
     <row r="74" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P74" s="19"/>
-      <c r="R74" s="19"/>
+      <c r="P74" s="16"/>
+      <c r="R74" s="16"/>
     </row>
     <row r="75" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P75" s="19"/>
-      <c r="R75" s="19"/>
+      <c r="P75" s="16"/>
+      <c r="R75" s="16"/>
     </row>
     <row r="76" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P76" s="19"/>
-      <c r="R76" s="19"/>
+      <c r="P76" s="16"/>
+      <c r="R76" s="16"/>
     </row>
     <row r="77" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P77" s="19"/>
-      <c r="R77" s="19"/>
+      <c r="P77" s="16"/>
+      <c r="R77" s="16"/>
     </row>
     <row r="78" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P78" s="19"/>
-      <c r="R78" s="19"/>
+      <c r="P78" s="16"/>
+      <c r="R78" s="16"/>
     </row>
     <row r="79" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P79" s="19"/>
-      <c r="R79" s="19"/>
+      <c r="P79" s="16"/>
+      <c r="R79" s="16"/>
     </row>
     <row r="80" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P80" s="19"/>
-      <c r="R80" s="19"/>
+      <c r="P80" s="16"/>
+      <c r="R80" s="16"/>
     </row>
     <row r="81" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P81" s="19"/>
-      <c r="R81" s="19"/>
+      <c r="P81" s="16"/>
+      <c r="R81" s="16"/>
     </row>
     <row r="82" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P82" s="19"/>
-      <c r="R82" s="19"/>
+      <c r="P82" s="16"/>
+      <c r="R82" s="16"/>
     </row>
     <row r="83" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P83" s="19"/>
-      <c r="R83" s="19"/>
+      <c r="P83" s="16"/>
+      <c r="R83" s="16"/>
     </row>
     <row r="84" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P84" s="19"/>
-      <c r="R84" s="19"/>
+      <c r="P84" s="16"/>
+      <c r="R84" s="16"/>
     </row>
     <row r="85" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P85" s="19"/>
-      <c r="R85" s="19"/>
+      <c r="P85" s="16"/>
+      <c r="R85" s="16"/>
     </row>
     <row r="86" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P86" s="19"/>
-      <c r="R86" s="19"/>
+      <c r="P86" s="16"/>
+      <c r="R86" s="16"/>
     </row>
     <row r="87" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P87" s="19"/>
-      <c r="R87" s="19"/>
+      <c r="P87" s="16"/>
+      <c r="R87" s="16"/>
     </row>
     <row r="88" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P88" s="19"/>
-      <c r="R88" s="19"/>
+      <c r="P88" s="16"/>
+      <c r="R88" s="16"/>
     </row>
     <row r="89" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P89" s="19"/>
-      <c r="R89" s="19"/>
+      <c r="P89" s="16"/>
+      <c r="R89" s="16"/>
     </row>
     <row r="90" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P90" s="19"/>
-      <c r="R90" s="19"/>
+      <c r="P90" s="16"/>
+      <c r="R90" s="16"/>
     </row>
     <row r="91" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P91" s="19"/>
-      <c r="R91" s="19"/>
+      <c r="P91" s="16"/>
+      <c r="R91" s="16"/>
     </row>
     <row r="92" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P92" s="19"/>
-      <c r="R92" s="19"/>
+      <c r="P92" s="16"/>
+      <c r="R92" s="16"/>
     </row>
     <row r="93" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P93" s="19"/>
-      <c r="R93" s="19"/>
+      <c r="P93" s="16"/>
+      <c r="R93" s="16"/>
     </row>
     <row r="94" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P94" s="19"/>
-      <c r="R94" s="19"/>
+      <c r="P94" s="16"/>
+      <c r="R94" s="16"/>
     </row>
     <row r="95" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P95" s="19"/>
-      <c r="R95" s="19"/>
+      <c r="P95" s="16"/>
+      <c r="R95" s="16"/>
     </row>
     <row r="96" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P96" s="19"/>
-      <c r="R96" s="19"/>
+      <c r="P96" s="16"/>
+      <c r="R96" s="16"/>
     </row>
     <row r="97" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P97" s="19"/>
-      <c r="R97" s="19"/>
+      <c r="P97" s="16"/>
+      <c r="R97" s="16"/>
     </row>
     <row r="98" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P98" s="19"/>
-      <c r="R98" s="19"/>
+      <c r="P98" s="16"/>
+      <c r="R98" s="16"/>
     </row>
     <row r="99" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P99" s="19"/>
-      <c r="R99" s="19"/>
+      <c r="P99" s="16"/>
+      <c r="R99" s="16"/>
     </row>
     <row r="100" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P100" s="19"/>
-      <c r="R100" s="19"/>
+      <c r="P100" s="16"/>
+      <c r="R100" s="16"/>
     </row>
     <row r="101" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P101" s="19"/>
-      <c r="R101" s="19"/>
+      <c r="P101" s="16"/>
+      <c r="R101" s="16"/>
     </row>
     <row r="102" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P102" s="19"/>
-      <c r="R102" s="19"/>
+      <c r="P102" s="16"/>
+      <c r="R102" s="16"/>
     </row>
     <row r="103" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P103" s="19"/>
-      <c r="R103" s="19"/>
+      <c r="P103" s="16"/>
+      <c r="R103" s="16"/>
     </row>
     <row r="104" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P104" s="19"/>
-      <c r="R104" s="19"/>
+      <c r="P104" s="16"/>
+      <c r="R104" s="16"/>
     </row>
     <row r="105" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P105" s="19"/>
-      <c r="R105" s="19"/>
+      <c r="P105" s="16"/>
+      <c r="R105" s="16"/>
     </row>
     <row r="106" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P106" s="19"/>
-      <c r="R106" s="19"/>
+      <c r="P106" s="16"/>
+      <c r="R106" s="16"/>
     </row>
     <row r="107" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P107" s="19"/>
-      <c r="R107" s="19"/>
+      <c r="P107" s="16"/>
+      <c r="R107" s="16"/>
     </row>
     <row r="108" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P108" s="19"/>
-      <c r="R108" s="19"/>
+      <c r="P108" s="16"/>
+      <c r="R108" s="16"/>
     </row>
     <row r="109" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P109" s="19"/>
-      <c r="R109" s="19"/>
+      <c r="P109" s="16"/>
+      <c r="R109" s="16"/>
     </row>
     <row r="110" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P110" s="19"/>
-      <c r="R110" s="19"/>
+      <c r="P110" s="16"/>
+      <c r="R110" s="16"/>
     </row>
     <row r="111" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P111" s="19"/>
-      <c r="R111" s="19"/>
+      <c r="P111" s="16"/>
+      <c r="R111" s="16"/>
     </row>
     <row r="112" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P112" s="19"/>
-      <c r="R112" s="19"/>
+      <c r="P112" s="16"/>
+      <c r="R112" s="16"/>
     </row>
     <row r="113" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P113" s="19"/>
-      <c r="R113" s="19"/>
+      <c r="P113" s="16"/>
+      <c r="R113" s="16"/>
     </row>
     <row r="114" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P114" s="19"/>
-      <c r="R114" s="19"/>
+      <c r="P114" s="16"/>
+      <c r="R114" s="16"/>
     </row>
     <row r="115" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P115" s="19"/>
-      <c r="R115" s="19"/>
+      <c r="P115" s="16"/>
+      <c r="R115" s="16"/>
     </row>
     <row r="116" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P116" s="19"/>
-      <c r="R116" s="19"/>
+      <c r="P116" s="16"/>
+      <c r="R116" s="16"/>
     </row>
     <row r="117" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P117" s="19"/>
-      <c r="R117" s="19"/>
+      <c r="P117" s="16"/>
+      <c r="R117" s="16"/>
     </row>
     <row r="118" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P118" s="19"/>
-      <c r="R118" s="19"/>
+      <c r="P118" s="16"/>
+      <c r="R118" s="16"/>
     </row>
     <row r="119" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P119" s="19"/>
-      <c r="R119" s="19"/>
+      <c r="P119" s="16"/>
+      <c r="R119" s="16"/>
     </row>
     <row r="120" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P120" s="19"/>
-      <c r="R120" s="19"/>
+      <c r="P120" s="16"/>
+      <c r="R120" s="16"/>
     </row>
     <row r="121" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P121" s="19"/>
-      <c r="R121" s="19"/>
+      <c r="P121" s="16"/>
+      <c r="R121" s="16"/>
     </row>
     <row r="122" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P122" s="19"/>
-      <c r="R122" s="19"/>
+      <c r="P122" s="16"/>
+      <c r="R122" s="16"/>
     </row>
     <row r="123" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P123" s="19"/>
-      <c r="R123" s="19"/>
+      <c r="P123" s="16"/>
+      <c r="R123" s="16"/>
     </row>
     <row r="124" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P124" s="19"/>
-      <c r="R124" s="19"/>
+      <c r="P124" s="16"/>
+      <c r="R124" s="16"/>
     </row>
     <row r="125" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P125" s="19"/>
-      <c r="R125" s="19"/>
+      <c r="P125" s="16"/>
+      <c r="R125" s="16"/>
     </row>
     <row r="126" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P126" s="19"/>
-      <c r="R126" s="19"/>
+      <c r="P126" s="16"/>
+      <c r="R126" s="16"/>
     </row>
     <row r="127" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P127" s="19"/>
-      <c r="R127" s="19"/>
+      <c r="P127" s="16"/>
+      <c r="R127" s="16"/>
     </row>
     <row r="128" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P128" s="19"/>
-      <c r="R128" s="19"/>
+      <c r="P128" s="16"/>
+      <c r="R128" s="16"/>
     </row>
     <row r="129" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P129" s="19"/>
-      <c r="R129" s="19"/>
+      <c r="P129" s="16"/>
+      <c r="R129" s="16"/>
     </row>
     <row r="130" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P130" s="19"/>
-      <c r="R130" s="19"/>
+      <c r="P130" s="16"/>
+      <c r="R130" s="16"/>
     </row>
     <row r="131" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P131" s="19"/>
-      <c r="R131" s="19"/>
+      <c r="P131" s="16"/>
+      <c r="R131" s="16"/>
     </row>
     <row r="132" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P132" s="19"/>
-      <c r="R132" s="19"/>
+      <c r="P132" s="16"/>
+      <c r="R132" s="16"/>
     </row>
     <row r="133" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P133" s="19"/>
-      <c r="R133" s="19"/>
+      <c r="P133" s="16"/>
+      <c r="R133" s="16"/>
     </row>
     <row r="134" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P134" s="19"/>
-      <c r="R134" s="19"/>
+      <c r="P134" s="16"/>
+      <c r="R134" s="16"/>
     </row>
     <row r="135" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P135" s="19"/>
-      <c r="R135" s="19"/>
+      <c r="P135" s="16"/>
+      <c r="R135" s="16"/>
     </row>
     <row r="136" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P136" s="19"/>
-      <c r="R136" s="19"/>
+      <c r="P136" s="16"/>
+      <c r="R136" s="16"/>
     </row>
     <row r="137" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P137" s="19"/>
-      <c r="R137" s="19"/>
+      <c r="P137" s="16"/>
+      <c r="R137" s="16"/>
     </row>
     <row r="138" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P138" s="19"/>
-      <c r="R138" s="19"/>
+      <c r="P138" s="16"/>
+      <c r="R138" s="16"/>
     </row>
     <row r="139" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P139" s="19"/>
-      <c r="R139" s="19"/>
+      <c r="P139" s="16"/>
+      <c r="R139" s="16"/>
     </row>
     <row r="140" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P140" s="19"/>
-      <c r="R140" s="19"/>
+      <c r="P140" s="16"/>
+      <c r="R140" s="16"/>
     </row>
     <row r="141" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P141" s="19"/>
-      <c r="R141" s="19"/>
+      <c r="P141" s="16"/>
+      <c r="R141" s="16"/>
     </row>
     <row r="142" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P142" s="19"/>
-      <c r="R142" s="19"/>
+      <c r="P142" s="16"/>
+      <c r="R142" s="16"/>
     </row>
     <row r="143" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P143" s="19"/>
-      <c r="R143" s="19"/>
+      <c r="P143" s="16"/>
+      <c r="R143" s="16"/>
     </row>
     <row r="144" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P144" s="19"/>
-      <c r="R144" s="19"/>
+      <c r="P144" s="16"/>
+      <c r="R144" s="16"/>
     </row>
     <row r="145" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P145" s="19"/>
-      <c r="R145" s="19"/>
+      <c r="P145" s="16"/>
+      <c r="R145" s="16"/>
     </row>
     <row r="146" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P146" s="19"/>
-      <c r="R146" s="19"/>
+      <c r="P146" s="16"/>
+      <c r="R146" s="16"/>
     </row>
     <row r="147" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P147" s="19"/>
-      <c r="R147" s="19"/>
+      <c r="P147" s="16"/>
+      <c r="R147" s="16"/>
     </row>
     <row r="148" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P148" s="19"/>
-      <c r="R148" s="19"/>
+      <c r="P148" s="16"/>
+      <c r="R148" s="16"/>
     </row>
     <row r="149" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P149" s="19"/>
-      <c r="R149" s="19"/>
+      <c r="P149" s="16"/>
+      <c r="R149" s="16"/>
     </row>
     <row r="150" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P150" s="19"/>
-      <c r="R150" s="19"/>
+      <c r="P150" s="16"/>
+      <c r="R150" s="16"/>
     </row>
     <row r="151" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P151" s="19"/>
-      <c r="R151" s="19"/>
+      <c r="P151" s="16"/>
+      <c r="R151" s="16"/>
     </row>
     <row r="152" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P152" s="19"/>
-      <c r="R152" s="19"/>
+      <c r="P152" s="16"/>
+      <c r="R152" s="16"/>
     </row>
     <row r="153" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P153" s="19"/>
-      <c r="R153" s="19"/>
+      <c r="P153" s="16"/>
+      <c r="R153" s="16"/>
     </row>
     <row r="154" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P154" s="19"/>
-      <c r="R154" s="19"/>
+      <c r="P154" s="16"/>
+      <c r="R154" s="16"/>
     </row>
     <row r="155" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P155" s="19"/>
-      <c r="R155" s="19"/>
+      <c r="P155" s="16"/>
+      <c r="R155" s="16"/>
     </row>
     <row r="156" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="R156" s="19"/>
+      <c r="R156" s="16"/>
     </row>
     <row r="157" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="R157" s="19"/>
+      <c r="R157" s="16"/>
     </row>
     <row r="158" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="R158" s="19"/>
+      <c r="R158" s="16"/>
     </row>
     <row r="159" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="R159" s="19"/>
+      <c r="R159" s="16"/>
     </row>
     <row r="160" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="R160" s="19"/>
+      <c r="R160" s="16"/>
     </row>
     <row r="161" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R161" s="19"/>
+      <c r="R161" s="16"/>
     </row>
     <row r="162" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R162" s="19"/>
+      <c r="R162" s="16"/>
     </row>
     <row r="163" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R163" s="19"/>
+      <c r="R163" s="16"/>
     </row>
     <row r="164" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R164" s="19"/>
+      <c r="R164" s="16"/>
     </row>
     <row r="165" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R165" s="19"/>
+      <c r="R165" s="16"/>
     </row>
     <row r="166" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R166" s="19"/>
+      <c r="R166" s="16"/>
     </row>
     <row r="167" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R167" s="19"/>
+      <c r="R167" s="16"/>
     </row>
     <row r="168" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R168" s="19"/>
+      <c r="R168" s="16"/>
     </row>
     <row r="169" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R169" s="19"/>
+      <c r="R169" s="16"/>
     </row>
     <row r="170" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R170" s="19"/>
+      <c r="R170" s="16"/>
     </row>
     <row r="171" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R171" s="19"/>
+      <c r="R171" s="16"/>
     </row>
     <row r="172" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R172" s="19"/>
+      <c r="R172" s="16"/>
     </row>
     <row r="173" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R173" s="19"/>
+      <c r="R173" s="16"/>
     </row>
     <row r="174" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R174" s="19"/>
+      <c r="R174" s="16"/>
     </row>
     <row r="175" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R175" s="19"/>
+      <c r="R175" s="16"/>
     </row>
     <row r="176" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R176" s="19"/>
+      <c r="R176" s="16"/>
     </row>
     <row r="177" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R177" s="19"/>
+      <c r="R177" s="16"/>
     </row>
     <row r="178" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R178" s="19"/>
+      <c r="R178" s="16"/>
     </row>
     <row r="179" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R179" s="19"/>
+      <c r="R179" s="16"/>
     </row>
     <row r="180" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R180" s="19"/>
+      <c r="R180" s="16"/>
     </row>
     <row r="181" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R181" s="19"/>
+      <c r="R181" s="16"/>
     </row>
     <row r="182" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R182" s="19"/>
+      <c r="R182" s="16"/>
     </row>
     <row r="183" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R183" s="19"/>
+      <c r="R183" s="16"/>
     </row>
     <row r="184" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R184" s="19"/>
+      <c r="R184" s="16"/>
     </row>
     <row r="185" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R185" s="19"/>
+      <c r="R185" s="16"/>
     </row>
     <row r="186" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R186" s="19"/>
+      <c r="R186" s="16"/>
     </row>
     <row r="187" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R187" s="19"/>
+      <c r="R187" s="16"/>
     </row>
     <row r="188" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R188" s="19"/>
+      <c r="R188" s="16"/>
     </row>
     <row r="189" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R189" s="19"/>
+      <c r="R189" s="16"/>
     </row>
     <row r="190" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R190" s="19"/>
+      <c r="R190" s="16"/>
     </row>
     <row r="191" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R191" s="19"/>
+      <c r="R191" s="16"/>
     </row>
     <row r="192" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R192" s="19"/>
+      <c r="R192" s="16"/>
     </row>
     <row r="193" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R193" s="19"/>
+      <c r="R193" s="16"/>
     </row>
     <row r="194" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R194" s="19"/>
+      <c r="R194" s="16"/>
     </row>
     <row r="195" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R195" s="19"/>
+      <c r="R195" s="16"/>
     </row>
     <row r="196" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R196" s="19"/>
+      <c r="R196" s="16"/>
     </row>
     <row r="197" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R197" s="19"/>
+      <c r="R197" s="16"/>
     </row>
     <row r="198" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R198" s="19"/>
+      <c r="R198" s="16"/>
     </row>
     <row r="199" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R199" s="19"/>
+      <c r="R199" s="16"/>
     </row>
     <row r="200" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R200" s="19"/>
+      <c r="R200" s="16"/>
     </row>
     <row r="201" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R201" s="19"/>
+      <c r="R201" s="16"/>
     </row>
     <row r="202" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R202" s="19"/>
+      <c r="R202" s="16"/>
     </row>
     <row r="203" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R203" s="19"/>
+      <c r="R203" s="16"/>
     </row>
     <row r="204" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R204" s="19"/>
+      <c r="R204" s="16"/>
     </row>
     <row r="205" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R205" s="19"/>
+      <c r="R205" s="16"/>
     </row>
     <row r="206" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R206" s="19"/>
+      <c r="R206" s="16"/>
     </row>
     <row r="207" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R207" s="19"/>
+      <c r="R207" s="16"/>
     </row>
     <row r="208" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R208" s="19"/>
+      <c r="R208" s="16"/>
     </row>
     <row r="209" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R209" s="19"/>
+      <c r="R209" s="16"/>
     </row>
     <row r="210" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R210" s="19"/>
+      <c r="R210" s="16"/>
     </row>
     <row r="211" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R211" s="19"/>
+      <c r="R211" s="16"/>
     </row>
     <row r="212" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R212" s="19"/>
+      <c r="R212" s="16"/>
     </row>
     <row r="213" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R213" s="19"/>
+      <c r="R213" s="16"/>
     </row>
     <row r="214" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R214" s="19"/>
+      <c r="R214" s="16"/>
     </row>
     <row r="215" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R215" s="19"/>
+      <c r="R215" s="16"/>
     </row>
     <row r="216" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R216" s="19"/>
+      <c r="R216" s="16"/>
     </row>
     <row r="217" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R217" s="19"/>
+      <c r="R217" s="16"/>
     </row>
     <row r="218" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R218" s="19"/>
+      <c r="R218" s="16"/>
     </row>
     <row r="219" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R219" s="19"/>
+      <c r="R219" s="16"/>
     </row>
     <row r="220" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R220" s="19"/>
+      <c r="R220" s="16"/>
     </row>
     <row r="221" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R221" s="19"/>
+      <c r="R221" s="16"/>
     </row>
     <row r="222" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R222" s="19"/>
+      <c r="R222" s="16"/>
     </row>
     <row r="223" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R223" s="19"/>
+      <c r="R223" s="16"/>
     </row>
     <row r="224" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R224" s="19"/>
+      <c r="R224" s="16"/>
     </row>
     <row r="225" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R225" s="19"/>
+      <c r="R225" s="16"/>
     </row>
     <row r="226" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R226" s="19"/>
+      <c r="R226" s="16"/>
     </row>
     <row r="227" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R227" s="19"/>
+      <c r="R227" s="16"/>
     </row>
     <row r="228" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R228" s="19"/>
+      <c r="R228" s="16"/>
     </row>
     <row r="229" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R229" s="19"/>
+      <c r="R229" s="16"/>
     </row>
     <row r="230" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R230" s="19"/>
+      <c r="R230" s="16"/>
     </row>
     <row r="231" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R231" s="19"/>
+      <c r="R231" s="16"/>
     </row>
     <row r="232" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R232" s="19"/>
+      <c r="R232" s="16"/>
     </row>
     <row r="233" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R233" s="19"/>
+      <c r="R233" s="16"/>
     </row>
     <row r="234" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R234" s="19"/>
+      <c r="R234" s="16"/>
     </row>
     <row r="235" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R235" s="19"/>
+      <c r="R235" s="16"/>
     </row>
     <row r="236" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R236" s="19"/>
+      <c r="R236" s="16"/>
     </row>
     <row r="237" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R237" s="19"/>
+      <c r="R237" s="16"/>
     </row>
     <row r="238" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R238" s="19"/>
+      <c r="R238" s="16"/>
     </row>
     <row r="239" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R239" s="19"/>
+      <c r="R239" s="16"/>
     </row>
     <row r="240" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R240" s="19"/>
+      <c r="R240" s="16"/>
     </row>
     <row r="241" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R241" s="19"/>
+      <c r="R241" s="16"/>
     </row>
     <row r="242" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R242" s="19"/>
+      <c r="R242" s="16"/>
     </row>
     <row r="243" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R243" s="19"/>
+      <c r="R243" s="16"/>
     </row>
     <row r="244" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R244" s="19"/>
+      <c r="R244" s="16"/>
     </row>
     <row r="245" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R245" s="19"/>
+      <c r="R245" s="16"/>
     </row>
     <row r="246" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R246" s="19"/>
+      <c r="R246" s="16"/>
     </row>
     <row r="247" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R247" s="19"/>
+      <c r="R247" s="16"/>
     </row>
     <row r="248" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R248" s="19"/>
+      <c r="R248" s="16"/>
     </row>
     <row r="249" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R249" s="19"/>
+      <c r="R249" s="16"/>
     </row>
     <row r="250" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R250" s="19"/>
+      <c r="R250" s="16"/>
     </row>
     <row r="251" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R251" s="19"/>
+      <c r="R251" s="16"/>
     </row>
     <row r="252" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R252" s="19"/>
+      <c r="R252" s="16"/>
     </row>
     <row r="253" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R253" s="19"/>
+      <c r="R253" s="16"/>
     </row>
     <row r="254" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R254" s="19"/>
+      <c r="R254" s="16"/>
     </row>
     <row r="255" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R255" s="19"/>
+      <c r="R255" s="16"/>
     </row>
     <row r="256" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R256" s="19"/>
+      <c r="R256" s="16"/>
     </row>
     <row r="257" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R257" s="19"/>
+      <c r="R257" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>